<commit_message>
added parallel execution for onf the tests
</commit_message>
<xml_diff>
--- a/src/test/testData/icdata.xlsx
+++ b/src/test/testData/icdata.xlsx
@@ -22,16 +22,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t xml:space="preserve">searchText</t>
+    <t xml:space="preserve">status</t>
   </si>
   <si>
-    <t xml:space="preserve">result</t>
+    <t xml:space="preserve">available</t>
   </si>
   <si>
-    <t xml:space="preserve">jenkins</t>
+    <t xml:space="preserve">pending</t>
   </si>
   <si>
-    <t xml:space="preserve">pine</t>
+    <t xml:space="preserve">sold</t>
   </si>
 </sst>
 </file>
@@ -129,40 +129,36 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.7"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="n">
-        <v>5</v>
-      </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>3</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>